<commit_message>
Save local changes before pull
</commit_message>
<xml_diff>
--- a/tickets.xlsx
+++ b/tickets.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -902,6 +902,43 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SAP Hana</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ramya</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Login being denied</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Trying to login but my credentials are denied.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Thats becoz some caps issue in login credentials . pls try andain and let me know if it persists.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>